<commit_message>
updating info for the supplement;
</commit_message>
<xml_diff>
--- a/mouse_proteomics/plotting_protein_changes.xlsx
+++ b/mouse_proteomics/plotting_protein_changes.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenniferwilson/Documents/phagocytosis_beta2Agonists/mouse_proteomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F7AF7A-B55B-4941-B771-25ED6F5E3D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C25681-862E-8749-854E-EDD94E06638D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3380" yWindow="5080" windowWidth="25660" windowHeight="19120" xr2:uid="{9A9BF76C-7D80-1D4C-BA5C-5A3634190ECD}"/>
+    <workbookView xWindow="3260" yWindow="6960" windowWidth="25660" windowHeight="19120" xr2:uid="{9A9BF76C-7D80-1D4C-BA5C-5A3634190ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -12078,7 +12078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B75E29F-BF9B-E54D-A877-1E42A23EB308}">
   <dimension ref="C3:E177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="U156" sqref="U156"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updating to reflect the most recent version of the paper
</commit_message>
<xml_diff>
--- a/mouse_proteomics/plotting_protein_changes.xlsx
+++ b/mouse_proteomics/plotting_protein_changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenniferwilson/Documents/phagocytosis_beta2Agonists/mouse_proteomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990A0332-AF9D-F540-BF7F-3B0597C778EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9542FFEC-9256-3E45-8E2B-8E51A991E525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4760" yWindow="520" windowWidth="33820" windowHeight="29220" xr2:uid="{9A9BF76C-7D80-1D4C-BA5C-5A3634190ECD}"/>
+    <workbookView xWindow="360" yWindow="500" windowWidth="33820" windowHeight="20380" xr2:uid="{9A9BF76C-7D80-1D4C-BA5C-5A3634190ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -8836,7 +8836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B75E29F-BF9B-E54D-A877-1E42A23EB308}">
   <dimension ref="C1:E124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD53"/>
     </sheetView>
   </sheetViews>

</xml_diff>